<commit_message>
Dummy commit to test credentials from WOAH
</commit_message>
<xml_diff>
--- a/data/PRRS.xlsx
+++ b/data/PRRS.xlsx
@@ -36353,7 +36353,12 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="39cfa7bf-be57-4825-ad81-4fa2c3988a7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="609b3323-4b9d-43ca-b8cd-8ed7d7422988" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -36367,8 +36372,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC53A90F68723D43865193287DBF125B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b951b4138421c1f6d18a2c1353684aac">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39cfa7bf-be57-4825-ad81-4fa2c3988a7d" xmlns:ns3="609b3323-4b9d-43ca-b8cd-8ed7d7422988" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dab20cd784e680407d684fca2e46b6f9" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC53A90F68723D43865193287DBF125B" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="33ffb581dd3a75a6cf30c4663109f26c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39cfa7bf-be57-4825-ad81-4fa2c3988a7d" xmlns:ns3="609b3323-4b9d-43ca-b8cd-8ed7d7422988" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c30450d24499608b5ac5f16aab9d7873" ns2:_="" ns3:_="">
     <xsd:import namespace="39cfa7bf-be57-4825-ad81-4fa2c3988a7d"/>
     <xsd:import namespace="609b3323-4b9d-43ca-b8cd-8ed7d7422988"/>
     <xsd:element name="properties">
@@ -36388,6 +36393,9 @@
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -36443,6 +36451,20 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ad0b2da7-f7f1-4ade-bc4d-78491eef27d0" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="22" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="609b3323-4b9d-43ca-b8cd-8ed7d7422988" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -36472,6 +36494,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{241053fb-da35-4cec-85da-3297fce3dbd1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="609b3323-4b9d-43ca-b8cd-8ed7d7422988">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -36591,5 +36624,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B105AF0-B7A3-4FEB-8ED6-F1A72E81BE9A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3B66314-746D-47A3-801C-BE09526BEC26}"/>
 </file>
</xml_diff>